<commit_message>
add data retrival file
</commit_message>
<xml_diff>
--- a/project/final_project/final_project_files/tables_info.xlsx
+++ b/project/final_project/final_project_files/tables_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalit\DataScience\project\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalit\DataScience\project\final_project\final_project_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CC133A-7768-4C53-B2D6-EFBA0FDA7E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CBB91A-2BEF-4E56-8DF3-E10E054A87C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7DB892FB-DC4A-4C12-8B0E-C1BFAB929BAF}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{7DB892FB-DC4A-4C12-8B0E-C1BFAB929BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -518,15 +518,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>23</xdr:col>
-          <xdr:colOff>254000</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>10886</xdr:rowOff>
+          <xdr:rowOff>17236</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>127907</xdr:colOff>
+          <xdr:colOff>121557</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>175986</xdr:rowOff>
+          <xdr:rowOff>182336</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -925,8 +925,8 @@
   <sheetPr codeName="גיליון1"/>
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1830,15 +1830,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>23</xdr:col>
-                <xdr:colOff>254000</xdr:colOff>
+                <xdr:colOff>247650</xdr:colOff>
                 <xdr:row>29</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>24</xdr:col>
-                <xdr:colOff>127000</xdr:colOff>
+                <xdr:colOff>120650</xdr:colOff>
                 <xdr:row>29</xdr:row>
-                <xdr:rowOff>177800</xdr:rowOff>
+                <xdr:rowOff>184150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>

</xml_diff>